<commit_message>
add RNAseq Analysis from CCBB
</commit_message>
<xml_diff>
--- a/Metasheet/PAXGene tubes frozen inv 28jun2019.xlsx
+++ b/Metasheet/PAXGene tubes frozen inv 28jun2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanju\Desktop\RNAseq\Metasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA48F31-9992-4CC5-953A-433F802AC997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBEF55B-E0DE-49C7-AE69-5D64D02EB4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="-13080" windowWidth="12150" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11295" yWindow="-13035" windowWidth="12150" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1314,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:W132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H131"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>